<commit_message>
Zeiterfassung 2. Versuch (Bitte nicht mehr überschreiben😭)
</commit_message>
<xml_diff>
--- a/Zeiterfassung Team 9.xlsx
+++ b/Zeiterfassung Team 9.xlsx
@@ -1,24 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10609"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luiskuehn/Downloads/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0C8E8709-F24E-354A-8FF0-43A443216326}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="480" yWindow="500" windowWidth="23920" windowHeight="13180" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Übersicht"/>
-    <sheet r:id="rId2" sheetId="2" name="Moritz Geiger"/>
-    <sheet r:id="rId3" sheetId="3" name="Robin Kraus"/>
-    <sheet r:id="rId4" sheetId="4" name="Luis Kühn"/>
-    <sheet r:id="rId5" sheetId="5" name="Hüma Yilmaz"/>
+    <sheet name="Übersicht" sheetId="1" r:id="rId1"/>
+    <sheet name="Moritz Geiger" sheetId="2" r:id="rId2"/>
+    <sheet name="Robin Kraus" sheetId="3" r:id="rId3"/>
+    <sheet name="Luis Kühn" sheetId="4" r:id="rId4"/>
+    <sheet name="Hüma Yilmaz" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="143">
   <si>
     <t>KW</t>
   </si>
@@ -140,63 +159,15 @@
     <t>Thema und Entities festlegen, Aufgaben aufteilen</t>
   </si>
   <si>
-    <t>Exceptions</t>
-  </si>
-  <si>
-    <t>Exceptions geschrieben für bereits existierende Filme</t>
-  </si>
-  <si>
-    <t>Query-Builder</t>
-  </si>
-  <si>
-    <t>Anfang Query-Builder mit den gewählten Entities</t>
-  </si>
-  <si>
-    <t>DB</t>
-  </si>
-  <si>
-    <t>Create-Dateien für DB erstellen</t>
-  </si>
-  <si>
-    <t>Service</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Read und Write-Service fertiggestellt </t>
-  </si>
-  <si>
     <t>Bugfix</t>
   </si>
   <si>
-    <t>Exceptions in Service abgeändert</t>
-  </si>
-  <si>
-    <t>Fix bei Suche nach ID</t>
-  </si>
-  <si>
-    <t>Datenbank aufsetzen und Fehlersuche</t>
-  </si>
-  <si>
     <t>Postman</t>
   </si>
   <si>
-    <t>Einrichten von Postman + Testen</t>
-  </si>
-  <si>
-    <t>PlantUML</t>
-  </si>
-  <si>
-    <t>Diagramme erstellen, Projekthandbuch entwerfen</t>
-  </si>
-  <si>
     <t>Jenkins</t>
   </si>
   <si>
-    <t>Jenkins Image erstellen, Jenkinsfile bearbeiten</t>
-  </si>
-  <si>
-    <t>Job erstellen, Fehlersuche und Testen</t>
-  </si>
-  <si>
     <t>20. Mai</t>
   </si>
   <si>
@@ -417,13 +388,90 @@
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>Figma UI-Elemente anordnen, Login Seite erstellen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6. Mai </t>
+  </si>
+  <si>
+    <t>Design von Buttons, Text und Bilder (Farbe, Größe, Schrift)</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Login Formular Beginn</t>
+  </si>
+  <si>
+    <t>Buttons, Input Felder, Login Route</t>
+  </si>
+  <si>
+    <t>Anpassungen</t>
+  </si>
+  <si>
+    <t>Anpassung von Login-Container an Navbar, Button &amp; Container Design</t>
+  </si>
+  <si>
+    <t>Bugfix in Login Route</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Awesome Font Icon Bug Fix und Textanpassung </t>
+  </si>
+  <si>
+    <t>Error-Handling bei fehlenden Büchern und keiner Verbindung zu API</t>
+  </si>
+  <si>
+    <t>26. Mai</t>
+  </si>
+  <si>
+    <t>Styling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CSS-Klassen für Suchformular hinzugefügt </t>
+  </si>
+  <si>
+    <t>27. Mai</t>
+  </si>
+  <si>
+    <t>Suchformular fixieren, Navbar anpassen beim hovern</t>
+  </si>
+  <si>
+    <t>5. Juni</t>
+  </si>
+  <si>
+    <t>Bugfix bei Error-Handling für falsche Suchkriterien</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Padding für Bodyelemente beim Hovern hinzugefügt </t>
+  </si>
+  <si>
+    <t>19. Juni</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CSS-Klassen abgeändert und neu angelegt </t>
+  </si>
+  <si>
+    <t>21. Juni</t>
+  </si>
+  <si>
+    <t>Buttons mit gleichem Abstand schrumpfen lassen bei kleineren Dsiplays</t>
+  </si>
+  <si>
+    <t>Umbenennung von Buttons/Routes</t>
+  </si>
+  <si>
+    <t>26.</t>
+  </si>
+  <si>
+    <t>Schriftart, Schriftgröße, generelle Textanpassungen</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -463,7 +511,7 @@
       <b/>
       <i/>
       <sz val="14"/>
-      <color rgb="FFff0000"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -573,133 +621,136 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="40">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="6" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="8" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="7" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="8" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="6" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="5" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="16" applyNumberFormat="1" borderId="8" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="16" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="8" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="6" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="6" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="6" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="6" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="6" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="6" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="8" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="8" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="8" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="6" applyBorder="1" fontId="5" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -710,10 +761,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -751,71 +802,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -843,7 +894,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -866,11 +917,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -879,13 +930,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -895,7 +946,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -904,7 +955,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -913,7 +964,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -921,10 +972,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -989,103 +1040,103 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" style="19" width="16.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="38" width="15.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="39" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="16.33203125" style="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" style="38" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5" style="39" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="23.25">
+    <row r="1" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="B1" s="32">
         <v>9</v>
       </c>
       <c r="C1" s="33"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+    <row r="2" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="30"/>
       <c r="B2" s="31"/>
       <c r="C2" s="33"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="23.25">
+    <row r="3" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="20.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="C4" s="34">
         <v>25</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="20.25">
+    <row r="5" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
       <c r="C5" s="34">
         <v>29.5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="20.25">
+    <row r="6" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
       <c r="C6" s="35">
         <v>37.75</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="20.25">
+    <row r="7" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>131</v>
+        <v>115</v>
       </c>
       <c r="C7" s="36">
         <v>23</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+    <row r="8" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="30"/>
       <c r="B8" s="31"/>
       <c r="C8" s="33"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
+    <row r="9" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="30"/>
       <c r="B9" s="31"/>
       <c r="C9" s="33"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="23.25">
+    <row r="10" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="37" t="s">
-        <v>132</v>
+        <v>116</v>
       </c>
       <c r="B10" s="31"/>
       <c r="C10" s="33"/>
@@ -1096,7 +1147,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -1104,16 +1155,16 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" style="18" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="28" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="18" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="19" width="16.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="19" width="67.7192857142857" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="13.5" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5" style="28" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5" style="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="67.6640625" style="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1130,16 +1181,17 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row r="2" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5"/>
       <c r="B2" s="23"/>
       <c r="C2" s="24">
         <f>SUM(C3:C61)</f>
+        <v>25</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row r="3" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="10">
         <v>15</v>
       </c>
@@ -1156,7 +1208,7 @@
         <v>39</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row r="4" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="10">
         <v>16</v>
       </c>
@@ -1167,13 +1219,13 @@
         <v>1.5</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="10">
         <v>16</v>
       </c>
@@ -1184,13 +1236,13 @@
         <v>2</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="10">
         <v>16</v>
       </c>
@@ -1201,13 +1253,13 @@
         <v>2</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="10">
         <v>17</v>
       </c>
@@ -1218,13 +1270,13 @@
         <v>1.5</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="10">
         <v>17</v>
       </c>
@@ -1235,13 +1287,13 @@
         <v>0.5</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="10">
         <v>17</v>
       </c>
@@ -1252,13 +1304,13 @@
         <v>0.5</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="10">
         <v>17</v>
       </c>
@@ -1269,13 +1321,13 @@
         <v>0.5</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="10">
         <v>17</v>
       </c>
@@ -1286,13 +1338,13 @@
         <v>2.5</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="10">
         <v>17</v>
       </c>
@@ -1303,13 +1355,13 @@
         <v>4</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="10">
         <v>17</v>
       </c>
@@ -1320,13 +1372,13 @@
         <v>1.5</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="10">
         <v>17</v>
       </c>
@@ -1337,13 +1389,13 @@
         <v>2.5</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="10">
         <v>18</v>
       </c>
@@ -1354,13 +1406,13 @@
         <v>1</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="10">
         <v>18</v>
       </c>
@@ -1371,13 +1423,13 @@
         <v>2</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="10">
         <v>18</v>
       </c>
@@ -1388,314 +1440,314 @@
         <v>2</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="14"/>
       <c r="B18" s="26"/>
       <c r="C18" s="14"/>
       <c r="D18" s="13"/>
       <c r="E18" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+    <row r="19" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="14"/>
       <c r="B19" s="26"/>
       <c r="C19" s="14"/>
       <c r="D19" s="13"/>
       <c r="E19" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+    <row r="20" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="14"/>
       <c r="B20" s="26"/>
       <c r="C20" s="14"/>
       <c r="D20" s="13"/>
       <c r="E20" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+    <row r="21" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="14"/>
       <c r="B21" s="26"/>
       <c r="C21" s="14"/>
       <c r="D21" s="13"/>
       <c r="E21" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+    <row r="22" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="14"/>
       <c r="B22" s="26"/>
       <c r="C22" s="14"/>
       <c r="D22" s="13"/>
       <c r="E22" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+    <row r="23" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="14"/>
       <c r="B23" s="26"/>
       <c r="C23" s="14"/>
       <c r="D23" s="13"/>
       <c r="E23" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+    <row r="24" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="14"/>
       <c r="B24" s="26"/>
       <c r="C24" s="14"/>
       <c r="D24" s="13"/>
       <c r="E24" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
+    <row r="25" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="14"/>
       <c r="B25" s="26"/>
       <c r="C25" s="14"/>
       <c r="D25" s="13"/>
       <c r="E25" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
+    <row r="26" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="14"/>
       <c r="B26" s="26"/>
       <c r="C26" s="14"/>
       <c r="D26" s="13"/>
       <c r="E26" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
+    <row r="27" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="14"/>
       <c r="B27" s="26"/>
       <c r="C27" s="14"/>
       <c r="D27" s="13"/>
       <c r="E27" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
+    <row r="28" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="14"/>
       <c r="B28" s="26"/>
       <c r="C28" s="14"/>
       <c r="D28" s="13"/>
       <c r="E28" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
+    <row r="29" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="14"/>
       <c r="B29" s="26"/>
       <c r="C29" s="14"/>
       <c r="D29" s="13"/>
       <c r="E29" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
+    <row r="30" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="14"/>
       <c r="B30" s="26"/>
       <c r="C30" s="14"/>
       <c r="D30" s="13"/>
       <c r="E30" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
+    <row r="31" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="14"/>
       <c r="B31" s="26"/>
       <c r="C31" s="14"/>
       <c r="D31" s="13"/>
       <c r="E31" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
+    <row r="32" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="14"/>
       <c r="B32" s="26"/>
       <c r="C32" s="14"/>
       <c r="D32" s="13"/>
       <c r="E32" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
+    <row r="33" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="14"/>
       <c r="B33" s="26"/>
       <c r="C33" s="14"/>
       <c r="D33" s="13"/>
       <c r="E33" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
+    <row r="34" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="14"/>
       <c r="B34" s="26"/>
       <c r="C34" s="14"/>
       <c r="D34" s="13"/>
       <c r="E34" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
+    <row r="35" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="14"/>
       <c r="B35" s="26"/>
       <c r="C35" s="14"/>
       <c r="D35" s="13"/>
       <c r="E35" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
+    <row r="36" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="14"/>
       <c r="B36" s="26"/>
       <c r="C36" s="14"/>
       <c r="D36" s="13"/>
       <c r="E36" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
+    <row r="37" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="14"/>
       <c r="B37" s="26"/>
       <c r="C37" s="14"/>
       <c r="D37" s="13"/>
       <c r="E37" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
+    <row r="38" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="14"/>
       <c r="B38" s="26"/>
       <c r="C38" s="14"/>
       <c r="D38" s="13"/>
       <c r="E38" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
+    <row r="39" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="14"/>
       <c r="B39" s="26"/>
       <c r="C39" s="14"/>
       <c r="D39" s="13"/>
       <c r="E39" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
+    <row r="40" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="14"/>
       <c r="B40" s="26"/>
       <c r="C40" s="14"/>
       <c r="D40" s="13"/>
       <c r="E40" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
+    <row r="41" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="14"/>
       <c r="B41" s="26"/>
       <c r="C41" s="14"/>
       <c r="D41" s="13"/>
       <c r="E41" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
+    <row r="42" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="14"/>
       <c r="B42" s="26"/>
       <c r="C42" s="14"/>
       <c r="D42" s="13"/>
       <c r="E42" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
+    <row r="43" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="14"/>
       <c r="B43" s="26"/>
       <c r="C43" s="14"/>
       <c r="D43" s="13"/>
       <c r="E43" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
+    <row r="44" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="14"/>
       <c r="B44" s="26"/>
       <c r="C44" s="14"/>
       <c r="D44" s="13"/>
       <c r="E44" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
+    <row r="45" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="14"/>
       <c r="B45" s="26"/>
       <c r="C45" s="14"/>
       <c r="D45" s="13"/>
       <c r="E45" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75">
+    <row r="46" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="14"/>
       <c r="B46" s="26"/>
       <c r="C46" s="14"/>
       <c r="D46" s="13"/>
       <c r="E46" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75">
+    <row r="47" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="14"/>
       <c r="B47" s="26"/>
       <c r="C47" s="14"/>
       <c r="D47" s="13"/>
       <c r="E47" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75">
+    <row r="48" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="14"/>
       <c r="B48" s="26"/>
       <c r="C48" s="14"/>
       <c r="D48" s="13"/>
       <c r="E48" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18.75">
+    <row r="49" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="14"/>
       <c r="B49" s="26"/>
       <c r="C49" s="14"/>
       <c r="D49" s="13"/>
       <c r="E49" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18.75">
+    <row r="50" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="14"/>
       <c r="B50" s="26"/>
       <c r="C50" s="14"/>
       <c r="D50" s="13"/>
       <c r="E50" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18.75">
+    <row r="51" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="14"/>
       <c r="B51" s="26"/>
       <c r="C51" s="14"/>
       <c r="D51" s="13"/>
       <c r="E51" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18.75">
+    <row r="52" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="14"/>
       <c r="B52" s="26"/>
       <c r="C52" s="14"/>
       <c r="D52" s="13"/>
       <c r="E52" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="18.75">
+    <row r="53" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="14"/>
       <c r="B53" s="26"/>
       <c r="C53" s="14"/>
       <c r="D53" s="13"/>
       <c r="E53" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="18.75">
+    <row r="54" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="14"/>
       <c r="B54" s="26"/>
       <c r="C54" s="14"/>
       <c r="D54" s="13"/>
       <c r="E54" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="18.75">
+    <row r="55" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="14"/>
       <c r="B55" s="26"/>
       <c r="C55" s="14"/>
       <c r="D55" s="13"/>
       <c r="E55" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="18.75">
+    <row r="56" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="14"/>
       <c r="B56" s="26"/>
       <c r="C56" s="14"/>
       <c r="D56" s="13"/>
       <c r="E56" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="18.75">
+    <row r="57" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="14"/>
       <c r="B57" s="26"/>
       <c r="C57" s="14"/>
       <c r="D57" s="13"/>
       <c r="E57" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="18.75">
+    <row r="58" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="14"/>
       <c r="B58" s="26"/>
       <c r="C58" s="14"/>
       <c r="D58" s="13"/>
       <c r="E58" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="18.75">
+    <row r="59" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="14"/>
       <c r="B59" s="26"/>
       <c r="C59" s="14"/>
       <c r="D59" s="13"/>
       <c r="E59" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="18.75">
+    <row r="60" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="14"/>
       <c r="B60" s="26"/>
       <c r="C60" s="14"/>
       <c r="D60" s="13"/>
       <c r="E60" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="18.75">
+    <row r="61" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="14"/>
       <c r="B61" s="26"/>
       <c r="C61" s="27"/>
@@ -1708,7 +1760,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -1716,16 +1768,16 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" style="18" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="19" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="18" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="19" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="19" width="66.57642857142856" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="13.5" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5" style="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5" style="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="66.5" style="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="23.25">
+    <row r="1" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1742,16 +1794,17 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="21">
+    <row r="2" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5"/>
       <c r="B2" s="6"/>
       <c r="C2" s="7">
         <f>SUM(C3:C61)</f>
+        <v>37.75</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="20.25">
+    <row r="3" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="10">
         <v>18</v>
       </c>
@@ -1768,7 +1821,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="20.25">
+    <row r="4" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="10">
         <v>19</v>
       </c>
@@ -1785,7 +1838,7 @@
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="20.25">
+    <row r="5" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="10">
         <v>19</v>
       </c>
@@ -1802,92 +1855,92 @@
         <v>12</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="20.25">
+    <row r="6" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="10">
         <v>20</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="C6" s="10">
         <v>2</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="20.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="10">
         <v>21</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="C7" s="10">
         <v>1</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="20.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="10">
         <v>21</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="C8" s="12">
         <v>3.25</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="20.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="10">
         <v>22</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="C9" s="10">
         <v>2</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="20.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="10">
         <v>22</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="C10" s="12">
         <v>2.75</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="20.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="10">
         <v>23</v>
       </c>
@@ -1901,49 +1954,49 @@
         <v>38</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="20.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="10">
         <v>24</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="C12" s="12">
         <v>2.5</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="20.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="10">
         <v>24</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="C13" s="12">
         <v>2</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="20.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="10">
         <v>24</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="C14" s="10">
         <v>1</v>
@@ -1952,98 +2005,98 @@
         <v>38</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="20.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14">
         <v>25</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="C15" s="14">
         <v>2</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="29"/>
       <c r="B16" s="30" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="C16" s="29">
         <v>2.25</v>
       </c>
       <c r="D16" s="30" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="E16" s="30" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="20.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="14">
         <v>25</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="C17" s="14">
         <v>1</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="20.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="14">
         <v>25</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="C18" s="14">
         <v>1</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="20.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="14">
         <v>26</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="C19" s="14">
         <v>3.25</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="20.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="14">
         <v>26</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="C20" s="14">
         <v>1</v>
@@ -2052,15 +2105,15 @@
         <v>38</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="20.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="14">
         <v>26</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="C21" s="14">
         <v>2</v>
@@ -2069,283 +2122,283 @@
         <v>38</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="20.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="14"/>
       <c r="B22" s="11"/>
       <c r="C22" s="14"/>
       <c r="D22" s="13"/>
       <c r="E22" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="20.25">
+    <row r="23" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="14"/>
       <c r="B23" s="11"/>
       <c r="C23" s="14"/>
       <c r="D23" s="13"/>
       <c r="E23" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="20.25">
+    <row r="24" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="14"/>
       <c r="B24" s="11"/>
       <c r="C24" s="14"/>
       <c r="D24" s="13"/>
       <c r="E24" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="20.25">
+    <row r="25" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="14"/>
       <c r="B25" s="11"/>
       <c r="C25" s="31"/>
       <c r="D25" s="13"/>
       <c r="E25" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="20.25">
+    <row r="26" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="14"/>
       <c r="B26" s="11"/>
       <c r="C26" s="14"/>
       <c r="D26" s="13"/>
       <c r="E26" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="20.25">
+    <row r="27" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="14"/>
       <c r="B27" s="11"/>
       <c r="C27" s="14"/>
       <c r="D27" s="13"/>
       <c r="E27" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
+    <row r="28" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="14"/>
       <c r="B28" s="11"/>
       <c r="C28" s="14"/>
       <c r="D28" s="13"/>
       <c r="E28" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
+    <row r="29" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="14"/>
       <c r="B29" s="11"/>
       <c r="C29" s="14"/>
       <c r="D29" s="13"/>
       <c r="E29" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
+    <row r="30" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="14"/>
       <c r="B30" s="11"/>
       <c r="C30" s="14"/>
       <c r="D30" s="13"/>
       <c r="E30" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
+    <row r="31" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="14"/>
       <c r="B31" s="11"/>
       <c r="C31" s="14"/>
       <c r="D31" s="13"/>
       <c r="E31" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
+    <row r="32" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="14"/>
       <c r="B32" s="11"/>
       <c r="C32" s="14"/>
       <c r="D32" s="13"/>
       <c r="E32" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
+    <row r="33" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="14"/>
       <c r="B33" s="11"/>
       <c r="C33" s="14"/>
       <c r="D33" s="13"/>
       <c r="E33" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
+    <row r="34" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="14"/>
       <c r="B34" s="11"/>
       <c r="C34" s="14"/>
       <c r="D34" s="13"/>
       <c r="E34" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
+    <row r="35" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="14"/>
       <c r="B35" s="11"/>
       <c r="C35" s="14"/>
       <c r="D35" s="13"/>
       <c r="E35" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
+    <row r="36" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="14"/>
       <c r="B36" s="11"/>
       <c r="C36" s="14"/>
       <c r="D36" s="13"/>
       <c r="E36" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
+    <row r="37" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="14"/>
       <c r="B37" s="11"/>
       <c r="C37" s="14"/>
       <c r="D37" s="13"/>
       <c r="E37" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
+    <row r="38" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="14"/>
       <c r="B38" s="11"/>
       <c r="C38" s="14"/>
       <c r="D38" s="13"/>
       <c r="E38" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
+    <row r="39" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="14"/>
       <c r="B39" s="11"/>
       <c r="C39" s="14"/>
       <c r="D39" s="13"/>
       <c r="E39" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
+    <row r="40" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="14"/>
       <c r="B40" s="11"/>
       <c r="C40" s="14"/>
       <c r="D40" s="13"/>
       <c r="E40" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
+    <row r="41" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="14"/>
       <c r="B41" s="11"/>
       <c r="C41" s="14"/>
       <c r="D41" s="13"/>
       <c r="E41" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
+    <row r="42" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="14"/>
       <c r="B42" s="11"/>
       <c r="C42" s="14"/>
       <c r="D42" s="13"/>
       <c r="E42" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
+    <row r="43" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="14"/>
       <c r="B43" s="11"/>
       <c r="C43" s="14"/>
       <c r="D43" s="13"/>
       <c r="E43" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
+    <row r="44" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="14"/>
       <c r="B44" s="11"/>
       <c r="C44" s="14"/>
       <c r="D44" s="13"/>
       <c r="E44" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
+    <row r="45" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="14"/>
       <c r="B45" s="11"/>
       <c r="C45" s="14"/>
       <c r="D45" s="13"/>
       <c r="E45" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75">
+    <row r="46" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="14"/>
       <c r="B46" s="11"/>
       <c r="C46" s="14"/>
       <c r="D46" s="13"/>
       <c r="E46" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75">
+    <row r="47" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="14"/>
       <c r="B47" s="11"/>
       <c r="C47" s="14"/>
       <c r="D47" s="13"/>
       <c r="E47" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75">
+    <row r="48" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="14"/>
       <c r="B48" s="11"/>
       <c r="C48" s="14"/>
       <c r="D48" s="13"/>
       <c r="E48" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18.75">
+    <row r="49" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="14"/>
       <c r="B49" s="11"/>
       <c r="C49" s="14"/>
       <c r="D49" s="13"/>
       <c r="E49" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18.75">
+    <row r="50" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="14"/>
       <c r="B50" s="11"/>
       <c r="C50" s="14"/>
       <c r="D50" s="13"/>
       <c r="E50" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18.75">
+    <row r="51" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="14"/>
       <c r="B51" s="11"/>
       <c r="C51" s="14"/>
       <c r="D51" s="13"/>
       <c r="E51" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18.75">
+    <row r="52" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="14"/>
       <c r="B52" s="11"/>
       <c r="C52" s="14"/>
       <c r="D52" s="13"/>
       <c r="E52" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="18.75">
+    <row r="53" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="14"/>
       <c r="B53" s="11"/>
       <c r="C53" s="14"/>
       <c r="D53" s="13"/>
       <c r="E53" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="18.75">
+    <row r="54" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="14"/>
       <c r="B54" s="11"/>
       <c r="C54" s="14"/>
       <c r="D54" s="13"/>
       <c r="E54" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="18.75">
+    <row r="55" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="14"/>
       <c r="B55" s="11"/>
       <c r="C55" s="14"/>
       <c r="D55" s="13"/>
       <c r="E55" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="18.75">
+    <row r="56" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="14"/>
       <c r="B56" s="11"/>
       <c r="C56" s="14"/>
       <c r="D56" s="13"/>
       <c r="E56" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="18.75">
+    <row r="57" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="14"/>
       <c r="B57" s="11"/>
       <c r="C57" s="14"/>
       <c r="D57" s="13"/>
       <c r="E57" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="18.75">
+    <row r="58" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="14"/>
       <c r="B58" s="11"/>
       <c r="C58" s="14"/>
       <c r="D58" s="13"/>
       <c r="E58" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="18.75">
+    <row r="59" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="14"/>
       <c r="B59" s="11"/>
       <c r="C59" s="14"/>
       <c r="D59" s="13"/>
       <c r="E59" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="18.75">
+    <row r="60" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="14"/>
       <c r="B60" s="11"/>
       <c r="C60" s="14"/>
       <c r="D60" s="13"/>
       <c r="E60" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="18.75">
+    <row r="61" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="14"/>
       <c r="B61" s="11"/>
       <c r="C61" s="27"/>
@@ -2358,7 +2411,625 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:E60"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.5" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5" style="28" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5" style="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="66.5" style="19" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="5"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="24">
+        <f>SUM(C3:C60)</f>
+        <v>30</v>
+      </c>
+      <c r="D2" s="8"/>
+      <c r="E2" s="9"/>
+    </row>
+    <row r="3" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="10">
+        <v>18</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="10">
+        <v>1.5</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="10">
+        <v>18</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>118</v>
+      </c>
+      <c r="C4" s="12">
+        <v>2</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="10">
+        <v>20</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="12">
+        <v>2</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="10">
+        <v>21</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="10">
+        <v>4</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="10">
+        <v>21</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" s="10">
+        <v>1.5</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="10">
+        <v>21</v>
+      </c>
+      <c r="B8" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="12">
+        <v>2</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="10">
+        <v>21</v>
+      </c>
+      <c r="B9" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" s="12">
+        <v>1</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="10">
+        <v>22</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="10">
+        <v>4</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="10">
+        <v>22</v>
+      </c>
+      <c r="B11" s="25" t="s">
+        <v>128</v>
+      </c>
+      <c r="C11" s="10">
+        <v>2</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="10">
+        <v>22</v>
+      </c>
+      <c r="B12" s="25" t="s">
+        <v>131</v>
+      </c>
+      <c r="C12" s="10">
+        <v>2</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="10">
+        <v>23</v>
+      </c>
+      <c r="B13" s="25" t="s">
+        <v>133</v>
+      </c>
+      <c r="C13" s="10">
+        <v>2</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="10">
+        <v>24</v>
+      </c>
+      <c r="B14" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="C14" s="10">
+        <v>1</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="14">
+        <v>25</v>
+      </c>
+      <c r="B15" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="C15" s="14">
+        <v>1</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="14">
+        <v>25</v>
+      </c>
+      <c r="B16" s="26" t="s">
+        <v>138</v>
+      </c>
+      <c r="C16" s="14">
+        <v>2</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="14">
+        <v>26</v>
+      </c>
+      <c r="B17" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="C17" s="14">
+        <v>1</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="B18" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="C18" s="14">
+        <v>1</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="14"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="9"/>
+    </row>
+    <row r="20" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="14"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="9"/>
+    </row>
+    <row r="21" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="14"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="9"/>
+    </row>
+    <row r="22" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="14"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="9"/>
+    </row>
+    <row r="23" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="14"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="9"/>
+    </row>
+    <row r="24" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="14"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="9"/>
+    </row>
+    <row r="25" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="14"/>
+      <c r="B25" s="26"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="9"/>
+    </row>
+    <row r="26" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="14"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="9"/>
+    </row>
+    <row r="27" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="14"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="9"/>
+    </row>
+    <row r="28" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="14"/>
+      <c r="B28" s="26"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="9"/>
+    </row>
+    <row r="29" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="14"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="9"/>
+    </row>
+    <row r="30" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="14"/>
+      <c r="B30" s="26"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="9"/>
+    </row>
+    <row r="31" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="14"/>
+      <c r="B31" s="26"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="9"/>
+    </row>
+    <row r="32" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="14"/>
+      <c r="B32" s="26"/>
+      <c r="C32" s="14"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="9"/>
+    </row>
+    <row r="33" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="14"/>
+      <c r="B33" s="26"/>
+      <c r="C33" s="14"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="9"/>
+    </row>
+    <row r="34" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="14"/>
+      <c r="B34" s="26"/>
+      <c r="C34" s="14"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="9"/>
+    </row>
+    <row r="35" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="14"/>
+      <c r="B35" s="26"/>
+      <c r="C35" s="14"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="9"/>
+    </row>
+    <row r="36" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="14"/>
+      <c r="B36" s="26"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="9"/>
+    </row>
+    <row r="37" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="14"/>
+      <c r="B37" s="26"/>
+      <c r="C37" s="14"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="9"/>
+    </row>
+    <row r="38" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="14"/>
+      <c r="B38" s="26"/>
+      <c r="C38" s="14"/>
+      <c r="D38" s="13"/>
+      <c r="E38" s="9"/>
+    </row>
+    <row r="39" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="14"/>
+      <c r="B39" s="26"/>
+      <c r="C39" s="14"/>
+      <c r="D39" s="13"/>
+      <c r="E39" s="9"/>
+    </row>
+    <row r="40" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="14"/>
+      <c r="B40" s="26"/>
+      <c r="C40" s="14"/>
+      <c r="D40" s="13"/>
+      <c r="E40" s="9"/>
+    </row>
+    <row r="41" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="14"/>
+      <c r="B41" s="26"/>
+      <c r="C41" s="14"/>
+      <c r="D41" s="13"/>
+      <c r="E41" s="9"/>
+    </row>
+    <row r="42" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="14"/>
+      <c r="B42" s="26"/>
+      <c r="C42" s="14"/>
+      <c r="D42" s="13"/>
+      <c r="E42" s="9"/>
+    </row>
+    <row r="43" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="14"/>
+      <c r="B43" s="26"/>
+      <c r="C43" s="14"/>
+      <c r="D43" s="13"/>
+      <c r="E43" s="9"/>
+    </row>
+    <row r="44" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="14"/>
+      <c r="B44" s="26"/>
+      <c r="C44" s="14"/>
+      <c r="D44" s="13"/>
+      <c r="E44" s="9"/>
+    </row>
+    <row r="45" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="14"/>
+      <c r="B45" s="26"/>
+      <c r="C45" s="14"/>
+      <c r="D45" s="13"/>
+      <c r="E45" s="9"/>
+    </row>
+    <row r="46" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="14"/>
+      <c r="B46" s="26"/>
+      <c r="C46" s="14"/>
+      <c r="D46" s="13"/>
+      <c r="E46" s="9"/>
+    </row>
+    <row r="47" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="14"/>
+      <c r="B47" s="26"/>
+      <c r="C47" s="14"/>
+      <c r="D47" s="13"/>
+      <c r="E47" s="9"/>
+    </row>
+    <row r="48" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="14"/>
+      <c r="B48" s="26"/>
+      <c r="C48" s="14"/>
+      <c r="D48" s="13"/>
+      <c r="E48" s="9"/>
+    </row>
+    <row r="49" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="14"/>
+      <c r="B49" s="26"/>
+      <c r="C49" s="14"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="9"/>
+    </row>
+    <row r="50" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="14"/>
+      <c r="B50" s="26"/>
+      <c r="C50" s="14"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="9"/>
+    </row>
+    <row r="51" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="14"/>
+      <c r="B51" s="26"/>
+      <c r="C51" s="14"/>
+      <c r="D51" s="13"/>
+      <c r="E51" s="9"/>
+    </row>
+    <row r="52" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="14"/>
+      <c r="B52" s="26"/>
+      <c r="C52" s="14"/>
+      <c r="D52" s="13"/>
+      <c r="E52" s="9"/>
+    </row>
+    <row r="53" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="14"/>
+      <c r="B53" s="26"/>
+      <c r="C53" s="14"/>
+      <c r="D53" s="13"/>
+      <c r="E53" s="9"/>
+    </row>
+    <row r="54" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="14"/>
+      <c r="B54" s="26"/>
+      <c r="C54" s="14"/>
+      <c r="D54" s="13"/>
+      <c r="E54" s="9"/>
+    </row>
+    <row r="55" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="14"/>
+      <c r="B55" s="26"/>
+      <c r="C55" s="14"/>
+      <c r="D55" s="13"/>
+      <c r="E55" s="9"/>
+    </row>
+    <row r="56" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="14"/>
+      <c r="B56" s="26"/>
+      <c r="C56" s="14"/>
+      <c r="D56" s="13"/>
+      <c r="E56" s="9"/>
+    </row>
+    <row r="57" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="14"/>
+      <c r="B57" s="26"/>
+      <c r="C57" s="14"/>
+      <c r="D57" s="13"/>
+      <c r="E57" s="9"/>
+    </row>
+    <row r="58" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="14"/>
+      <c r="B58" s="26"/>
+      <c r="C58" s="14"/>
+      <c r="D58" s="13"/>
+      <c r="E58" s="9"/>
+    </row>
+    <row r="59" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="14"/>
+      <c r="B59" s="26"/>
+      <c r="C59" s="14"/>
+      <c r="D59" s="13"/>
+      <c r="E59" s="9"/>
+    </row>
+    <row r="60" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="14"/>
+      <c r="B60" s="26"/>
+      <c r="C60" s="27"/>
+      <c r="D60" s="13"/>
+      <c r="E60" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -2366,617 +3037,43 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" style="18" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="28" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="18" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="19" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="19" width="66.57642857142856" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="13.5" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5" style="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5" style="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5" style="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="65.5" style="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="23.25">
+    <row r="1" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="21">
-      <c r="A2" s="5"/>
-      <c r="B2" s="23"/>
-      <c r="C2" s="24">
-        <f>SUM(C3:C60)</f>
-      </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="20.25">
-      <c r="A3" s="10">
-        <v>15</v>
-      </c>
-      <c r="B3" s="25">
-        <v>45392</v>
-      </c>
-      <c r="C3" s="10">
-        <v>1</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="20.25">
-      <c r="A4" s="10">
-        <v>16</v>
-      </c>
-      <c r="B4" s="25">
-        <v>45398</v>
-      </c>
-      <c r="C4" s="12">
-        <v>0.5</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="20.25">
-      <c r="A5" s="10">
-        <v>16</v>
-      </c>
-      <c r="B5" s="25">
-        <v>45400</v>
-      </c>
-      <c r="C5" s="12">
-        <v>1.5</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="20.25">
-      <c r="A6" s="10">
-        <v>16</v>
-      </c>
-      <c r="B6" s="25">
-        <v>45402</v>
-      </c>
-      <c r="C6" s="10">
-        <v>1</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="20.25">
-      <c r="A7" s="10">
-        <v>17</v>
-      </c>
-      <c r="B7" s="25">
-        <v>45404</v>
-      </c>
-      <c r="C7" s="10">
-        <v>2</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="20.25">
-      <c r="A8" s="10">
-        <v>17</v>
-      </c>
-      <c r="B8" s="25">
-        <v>45405</v>
-      </c>
-      <c r="C8" s="12">
-        <v>0.5</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="20.25">
-      <c r="A9" s="10">
-        <v>17</v>
-      </c>
-      <c r="B9" s="25">
-        <v>29</v>
-      </c>
-      <c r="C9" s="12">
-        <v>0.5</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="20.25">
-      <c r="A10" s="10">
-        <v>17</v>
-      </c>
-      <c r="B10" s="25">
-        <v>45406</v>
-      </c>
-      <c r="C10" s="10">
-        <v>3</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="20.25">
-      <c r="A11" s="10">
-        <v>17</v>
-      </c>
-      <c r="B11" s="25">
-        <v>45410</v>
-      </c>
-      <c r="C11" s="10">
-        <v>4</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="20.25">
-      <c r="A12" s="10">
-        <v>18</v>
-      </c>
-      <c r="B12" s="25">
-        <v>45411</v>
-      </c>
-      <c r="C12" s="10">
-        <v>4</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="20.25">
-      <c r="A13" s="10">
-        <v>18</v>
-      </c>
-      <c r="B13" s="25">
-        <v>45412</v>
-      </c>
-      <c r="C13" s="10">
-        <v>2</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="20.25">
-      <c r="A14" s="10">
-        <v>18</v>
-      </c>
-      <c r="B14" s="25">
-        <v>45413</v>
-      </c>
-      <c r="C14" s="10">
-        <v>2</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="20.25">
-      <c r="A15" s="14"/>
-      <c r="B15" s="26"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="20.25">
-      <c r="A16" s="14"/>
-      <c r="B16" s="26"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="20.25">
-      <c r="A17" s="14"/>
-      <c r="B17" s="26"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="20.25">
-      <c r="A18" s="14"/>
-      <c r="B18" s="26"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="20.25">
-      <c r="A19" s="14"/>
-      <c r="B19" s="26"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="20.25">
-      <c r="A20" s="14"/>
-      <c r="B20" s="26"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="20.25">
-      <c r="A21" s="14"/>
-      <c r="B21" s="26"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="20.25">
-      <c r="A22" s="14"/>
-      <c r="B22" s="26"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="20.25">
-      <c r="A23" s="14"/>
-      <c r="B23" s="26"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="20.25">
-      <c r="A24" s="14"/>
-      <c r="B24" s="26"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="20.25">
-      <c r="A25" s="14"/>
-      <c r="B25" s="26"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="20.25">
-      <c r="A26" s="14"/>
-      <c r="B26" s="26"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="20.25">
-      <c r="A27" s="14"/>
-      <c r="B27" s="26"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
-      <c r="A28" s="14"/>
-      <c r="B28" s="26"/>
-      <c r="C28" s="14"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
-      <c r="A29" s="14"/>
-      <c r="B29" s="26"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
-      <c r="A30" s="14"/>
-      <c r="B30" s="26"/>
-      <c r="C30" s="14"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
-      <c r="A31" s="14"/>
-      <c r="B31" s="26"/>
-      <c r="C31" s="14"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
-      <c r="A32" s="14"/>
-      <c r="B32" s="26"/>
-      <c r="C32" s="14"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
-      <c r="A33" s="14"/>
-      <c r="B33" s="26"/>
-      <c r="C33" s="14"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
-      <c r="A34" s="14"/>
-      <c r="B34" s="26"/>
-      <c r="C34" s="14"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
-      <c r="A35" s="14"/>
-      <c r="B35" s="26"/>
-      <c r="C35" s="14"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
-      <c r="A36" s="14"/>
-      <c r="B36" s="26"/>
-      <c r="C36" s="14"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
-      <c r="A37" s="14"/>
-      <c r="B37" s="26"/>
-      <c r="C37" s="14"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
-      <c r="A38" s="14"/>
-      <c r="B38" s="26"/>
-      <c r="C38" s="14"/>
-      <c r="D38" s="13"/>
-      <c r="E38" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
-      <c r="A39" s="14"/>
-      <c r="B39" s="26"/>
-      <c r="C39" s="14"/>
-      <c r="D39" s="13"/>
-      <c r="E39" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
-      <c r="A40" s="14"/>
-      <c r="B40" s="26"/>
-      <c r="C40" s="14"/>
-      <c r="D40" s="13"/>
-      <c r="E40" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
-      <c r="A41" s="14"/>
-      <c r="B41" s="26"/>
-      <c r="C41" s="14"/>
-      <c r="D41" s="13"/>
-      <c r="E41" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
-      <c r="A42" s="14"/>
-      <c r="B42" s="26"/>
-      <c r="C42" s="14"/>
-      <c r="D42" s="13"/>
-      <c r="E42" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
-      <c r="A43" s="14"/>
-      <c r="B43" s="26"/>
-      <c r="C43" s="14"/>
-      <c r="D43" s="13"/>
-      <c r="E43" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
-      <c r="A44" s="14"/>
-      <c r="B44" s="26"/>
-      <c r="C44" s="14"/>
-      <c r="D44" s="13"/>
-      <c r="E44" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
-      <c r="A45" s="14"/>
-      <c r="B45" s="26"/>
-      <c r="C45" s="14"/>
-      <c r="D45" s="13"/>
-      <c r="E45" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75">
-      <c r="A46" s="14"/>
-      <c r="B46" s="26"/>
-      <c r="C46" s="14"/>
-      <c r="D46" s="13"/>
-      <c r="E46" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75">
-      <c r="A47" s="14"/>
-      <c r="B47" s="26"/>
-      <c r="C47" s="14"/>
-      <c r="D47" s="13"/>
-      <c r="E47" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75">
-      <c r="A48" s="14"/>
-      <c r="B48" s="26"/>
-      <c r="C48" s="14"/>
-      <c r="D48" s="13"/>
-      <c r="E48" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18.75">
-      <c r="A49" s="14"/>
-      <c r="B49" s="26"/>
-      <c r="C49" s="14"/>
-      <c r="D49" s="13"/>
-      <c r="E49" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18.75">
-      <c r="A50" s="14"/>
-      <c r="B50" s="26"/>
-      <c r="C50" s="14"/>
-      <c r="D50" s="13"/>
-      <c r="E50" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18.75">
-      <c r="A51" s="14"/>
-      <c r="B51" s="26"/>
-      <c r="C51" s="14"/>
-      <c r="D51" s="13"/>
-      <c r="E51" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18.75">
-      <c r="A52" s="14"/>
-      <c r="B52" s="26"/>
-      <c r="C52" s="14"/>
-      <c r="D52" s="13"/>
-      <c r="E52" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="18.75">
-      <c r="A53" s="14"/>
-      <c r="B53" s="26"/>
-      <c r="C53" s="14"/>
-      <c r="D53" s="13"/>
-      <c r="E53" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="18.75">
-      <c r="A54" s="14"/>
-      <c r="B54" s="26"/>
-      <c r="C54" s="14"/>
-      <c r="D54" s="13"/>
-      <c r="E54" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="18.75">
-      <c r="A55" s="14"/>
-      <c r="B55" s="26"/>
-      <c r="C55" s="14"/>
-      <c r="D55" s="13"/>
-      <c r="E55" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="18.75">
-      <c r="A56" s="14"/>
-      <c r="B56" s="26"/>
-      <c r="C56" s="14"/>
-      <c r="D56" s="13"/>
-      <c r="E56" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="18.75">
-      <c r="A57" s="14"/>
-      <c r="B57" s="26"/>
-      <c r="C57" s="14"/>
-      <c r="D57" s="13"/>
-      <c r="E57" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="18.75">
-      <c r="A58" s="14"/>
-      <c r="B58" s="26"/>
-      <c r="C58" s="14"/>
-      <c r="D58" s="13"/>
-      <c r="E58" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="18.75">
-      <c r="A59" s="14"/>
-      <c r="B59" s="26"/>
-      <c r="C59" s="14"/>
-      <c r="D59" s="13"/>
-      <c r="E59" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="18.75">
-      <c r="A60" s="14"/>
-      <c r="B60" s="26"/>
-      <c r="C60" s="27"/>
-      <c r="D60" s="13"/>
-      <c r="E60" s="9"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:E60"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" style="18" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="19" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="20" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="19" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="19" width="65.57642857142856" customWidth="1" bestFit="1"/>
-  </cols>
-  <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="23.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="21">
+    <row r="2" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5"/>
       <c r="B2" s="6"/>
       <c r="C2" s="7">
         <f>SUM(C3:C60)</f>
+        <v>23</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="20.25">
+    <row r="3" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="10">
         <v>18</v>
       </c>
@@ -2993,7 +3090,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="20.25">
+    <row r="4" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="10">
         <v>19</v>
       </c>
@@ -3010,7 +3107,7 @@
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="20.25">
+    <row r="5" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="10">
         <v>19</v>
       </c>
@@ -3027,7 +3124,7 @@
         <v>12</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="20.25">
+    <row r="6" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="14">
         <v>22</v>
       </c>
@@ -3044,7 +3141,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="20.25">
+    <row r="7" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="14">
         <v>23</v>
       </c>
@@ -3061,7 +3158,7 @@
         <v>17</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row r="8" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="14">
         <v>23</v>
       </c>
@@ -3078,7 +3175,7 @@
         <v>20</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row r="9" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="14">
         <v>23</v>
       </c>
@@ -3095,7 +3192,7 @@
         <v>22</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row r="10" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="16">
         <v>24</v>
       </c>
@@ -3112,7 +3209,7 @@
         <v>24</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row r="11" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="14">
         <v>25</v>
       </c>
@@ -3129,7 +3226,7 @@
         <v>26</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row r="12" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="14">
         <v>25</v>
       </c>
@@ -3146,7 +3243,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row r="13" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="14">
         <v>25</v>
       </c>
@@ -3163,7 +3260,7 @@
         <v>31</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row r="14" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="14">
         <v>26</v>
       </c>
@@ -3180,7 +3277,7 @@
         <v>34</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row r="15" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14">
         <v>26</v>
       </c>
@@ -3197,7 +3294,7 @@
         <v>36</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+    <row r="16" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="14">
         <v>26</v>
       </c>
@@ -3214,7 +3311,7 @@
         <v>37</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+    <row r="17" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="14">
         <v>26</v>
       </c>
@@ -3231,301 +3328,301 @@
         <v>38</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+    <row r="18" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="14"/>
       <c r="B18" s="11"/>
       <c r="C18" s="15"/>
       <c r="D18" s="13"/>
       <c r="E18" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+    <row r="19" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="14"/>
       <c r="B19" s="11"/>
       <c r="C19" s="15"/>
       <c r="D19" s="13"/>
       <c r="E19" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+    <row r="20" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="14"/>
       <c r="B20" s="11"/>
       <c r="C20" s="15"/>
       <c r="D20" s="13"/>
       <c r="E20" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+    <row r="21" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="14"/>
       <c r="B21" s="11"/>
       <c r="C21" s="15"/>
       <c r="D21" s="13"/>
       <c r="E21" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+    <row r="22" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="14"/>
       <c r="B22" s="11"/>
       <c r="C22" s="15"/>
       <c r="D22" s="13"/>
       <c r="E22" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+    <row r="23" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="14"/>
       <c r="B23" s="11"/>
       <c r="C23" s="15"/>
       <c r="D23" s="13"/>
       <c r="E23" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+    <row r="24" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="14"/>
       <c r="B24" s="11"/>
       <c r="C24" s="15"/>
       <c r="D24" s="13"/>
       <c r="E24" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
+    <row r="25" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="14"/>
       <c r="B25" s="11"/>
       <c r="C25" s="15"/>
       <c r="D25" s="13"/>
       <c r="E25" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
+    <row r="26" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="14"/>
       <c r="B26" s="11"/>
       <c r="C26" s="15"/>
       <c r="D26" s="13"/>
       <c r="E26" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
+    <row r="27" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="14"/>
       <c r="B27" s="11"/>
       <c r="C27" s="15"/>
       <c r="D27" s="13"/>
       <c r="E27" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
+    <row r="28" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="14"/>
       <c r="B28" s="11"/>
       <c r="C28" s="15"/>
       <c r="D28" s="13"/>
       <c r="E28" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
+    <row r="29" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="14"/>
       <c r="B29" s="11"/>
       <c r="C29" s="15"/>
       <c r="D29" s="13"/>
       <c r="E29" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
+    <row r="30" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="14"/>
       <c r="B30" s="11"/>
       <c r="C30" s="15"/>
       <c r="D30" s="13"/>
       <c r="E30" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
+    <row r="31" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="14"/>
       <c r="B31" s="11"/>
       <c r="C31" s="15"/>
       <c r="D31" s="13"/>
       <c r="E31" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
+    <row r="32" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="14"/>
       <c r="B32" s="11"/>
       <c r="C32" s="15"/>
       <c r="D32" s="13"/>
       <c r="E32" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
+    <row r="33" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="14"/>
       <c r="B33" s="11"/>
       <c r="C33" s="15"/>
       <c r="D33" s="13"/>
       <c r="E33" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
+    <row r="34" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="14"/>
       <c r="B34" s="11"/>
       <c r="C34" s="15"/>
       <c r="D34" s="13"/>
       <c r="E34" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
+    <row r="35" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="14"/>
       <c r="B35" s="11"/>
       <c r="C35" s="15"/>
       <c r="D35" s="13"/>
       <c r="E35" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
+    <row r="36" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="14"/>
       <c r="B36" s="11"/>
       <c r="C36" s="15"/>
       <c r="D36" s="13"/>
       <c r="E36" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
+    <row r="37" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="14"/>
       <c r="B37" s="11"/>
       <c r="C37" s="15"/>
       <c r="D37" s="13"/>
       <c r="E37" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
+    <row r="38" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="14"/>
       <c r="B38" s="11"/>
       <c r="C38" s="15"/>
       <c r="D38" s="13"/>
       <c r="E38" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
+    <row r="39" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="14"/>
       <c r="B39" s="11"/>
       <c r="C39" s="15"/>
       <c r="D39" s="13"/>
       <c r="E39" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
+    <row r="40" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="14"/>
       <c r="B40" s="11"/>
       <c r="C40" s="15"/>
       <c r="D40" s="13"/>
       <c r="E40" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
+    <row r="41" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="14"/>
       <c r="B41" s="11"/>
       <c r="C41" s="15"/>
       <c r="D41" s="13"/>
       <c r="E41" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
+    <row r="42" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="14"/>
       <c r="B42" s="11"/>
       <c r="C42" s="15"/>
       <c r="D42" s="13"/>
       <c r="E42" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
+    <row r="43" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="14"/>
       <c r="B43" s="11"/>
       <c r="C43" s="15"/>
       <c r="D43" s="13"/>
       <c r="E43" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
+    <row r="44" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="14"/>
       <c r="B44" s="11"/>
       <c r="C44" s="15"/>
       <c r="D44" s="13"/>
       <c r="E44" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
+    <row r="45" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="14"/>
       <c r="B45" s="11"/>
       <c r="C45" s="15"/>
       <c r="D45" s="13"/>
       <c r="E45" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75">
+    <row r="46" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="14"/>
       <c r="B46" s="11"/>
       <c r="C46" s="15"/>
       <c r="D46" s="13"/>
       <c r="E46" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75">
+    <row r="47" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="14"/>
       <c r="B47" s="11"/>
       <c r="C47" s="15"/>
       <c r="D47" s="13"/>
       <c r="E47" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75">
+    <row r="48" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="14"/>
       <c r="B48" s="11"/>
       <c r="C48" s="15"/>
       <c r="D48" s="13"/>
       <c r="E48" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18.75">
+    <row r="49" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="14"/>
       <c r="B49" s="11"/>
       <c r="C49" s="15"/>
       <c r="D49" s="13"/>
       <c r="E49" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18.75">
+    <row r="50" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="14"/>
       <c r="B50" s="11"/>
       <c r="C50" s="15"/>
       <c r="D50" s="13"/>
       <c r="E50" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18.75">
+    <row r="51" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="14"/>
       <c r="B51" s="11"/>
       <c r="C51" s="15"/>
       <c r="D51" s="13"/>
       <c r="E51" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18.75">
+    <row r="52" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="14"/>
       <c r="B52" s="11"/>
       <c r="C52" s="15"/>
       <c r="D52" s="13"/>
       <c r="E52" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="18.75">
+    <row r="53" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="14"/>
       <c r="B53" s="11"/>
       <c r="C53" s="15"/>
       <c r="D53" s="13"/>
       <c r="E53" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="18.75">
+    <row r="54" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="14"/>
       <c r="B54" s="11"/>
       <c r="C54" s="15"/>
       <c r="D54" s="13"/>
       <c r="E54" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="18.75">
+    <row r="55" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="14"/>
       <c r="B55" s="11"/>
       <c r="C55" s="15"/>
       <c r="D55" s="13"/>
       <c r="E55" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="18.75">
+    <row r="56" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="14"/>
       <c r="B56" s="11"/>
       <c r="C56" s="15"/>
       <c r="D56" s="13"/>
       <c r="E56" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="18.75">
+    <row r="57" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="14"/>
       <c r="B57" s="11"/>
       <c r="C57" s="15"/>
       <c r="D57" s="13"/>
       <c r="E57" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="18.75">
+    <row r="58" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="14"/>
       <c r="B58" s="11"/>
       <c r="C58" s="15"/>
       <c r="D58" s="13"/>
       <c r="E58" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="18.75">
+    <row r="59" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="14"/>
       <c r="B59" s="11"/>
       <c r="C59" s="15"/>
       <c r="D59" s="13"/>
       <c r="E59" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="18.75">
+    <row r="60" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="14"/>
       <c r="B60" s="11"/>
       <c r="C60" s="17"/>

</xml_diff>